<commit_message>
daily orders with weekly summary
</commit_message>
<xml_diff>
--- a/src/JCSGYK/AdminBundle/Resources/public/reports/dailyorder.xlsx
+++ b/src/JCSGYK/AdminBundle/Resources/public/reports/dailyorder.xlsx
@@ -4,16 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9920" yWindow="1520" windowWidth="32880" windowHeight="22360"/>
+    <workbookView xWindow="21840" yWindow="2860" windowWidth="26580" windowHeight="18160"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
     <sheet name="Munka2" sheetId="2" r:id="rId2"/>
     <sheet name="Munka3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Munka1!$A$1:$I$18</definedName>
-  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t xml:space="preserve">Szociális Intézmények Gazdasági Hivatala </t>
   </si>
@@ -50,9 +47,6 @@
     <t>Józsefvárosi Szociális Szolgáltató és Gyermekjóléti Központ</t>
   </si>
   <si>
-    <t>MEGRENDELŐ</t>
-  </si>
-  <si>
     <t>A pót-és lerendelések levonása utáni kiküldendő adagszámok.</t>
   </si>
   <si>
@@ -78,6 +72,33 @@
   </si>
   <si>
     <t>[dailyorders.amount]</t>
+  </si>
+  <si>
+    <t>Adagszám</t>
+  </si>
+  <si>
+    <t>Egység ár</t>
+  </si>
+  <si>
+    <t>Fizetendő</t>
+  </si>
+  <si>
+    <t>Ebéd :</t>
+  </si>
+  <si>
+    <t>Számlázandó  :</t>
+  </si>
+  <si>
+    <t>[et.egysegar]</t>
+  </si>
+  <si>
+    <t>[et.fizetendo]</t>
+  </si>
+  <si>
+    <t>[et.adagszam;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[et.cim]</t>
   </si>
 </sst>
 </file>
@@ -88,7 +109,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;Ft&quot;_-;\-* #,##0.00\ &quot;Ft&quot;_-;_-* &quot;-&quot;??\ &quot;Ft&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;Ft&quot;_-;\-* #,##0\ &quot;Ft&quot;_-;_-* &quot;-&quot;??\ &quot;Ft&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial CE"/>
@@ -153,6 +174,12 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial CE"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,7 +190,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -186,8 +213,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="74">
+  <cellStyleXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -262,13 +326,34 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -293,15 +378,30 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="74">
+  <cellStyles count="98">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -339,6 +439,18 @@
     <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -375,6 +487,18 @@
     <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -774,15 +898,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="9" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
@@ -796,7 +919,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -811,7 +934,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -826,22 +949,22 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
+      <c r="A4" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
       <c r="A5" s="1"/>
@@ -855,17 +978,17 @@
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1">
-      <c r="A6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
+      <c r="A6" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1">
       <c r="A7" s="1"/>
@@ -879,17 +1002,17 @@
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1">
-      <c r="A8" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
+      <c r="A8" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
@@ -907,35 +1030,35 @@
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
-      <c r="A10" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="11"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5"/>
+      <c r="A10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="10"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="4"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1">
-      <c r="A11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="10" t="s">
+      <c r="A11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="6"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="5"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
@@ -962,42 +1085,54 @@
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="A15" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="16"/>
+      <c r="E15" s="17" t="s">
+        <v>23</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I15" s="1"/>
+      <c r="H15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1">
-      <c r="A16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="1"/>
+      <c r="A16" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="18" t="s">
+        <v>23</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1">
@@ -1012,16 +1147,18 @@
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1">
-      <c r="A18" s="1"/>
+      <c r="A18" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="9"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="9" t="s">
-        <v>9</v>
+      <c r="I18" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily Orders weekdays / weekend summary
</commit_message>
<xml_diff>
--- a/src/JCSGYK/AdminBundle/Resources/public/reports/dailyorder.xlsx
+++ b/src/JCSGYK/AdminBundle/Resources/public/reports/dailyorder.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="21840" yWindow="2860" windowWidth="26580" windowHeight="18160"/>
@@ -19,26 +19,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
-  <si>
-    <t xml:space="preserve">Szociális Intézmények Gazdasági Hivatala </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Budapest</t>
   </si>
   <si>
-    <t>Kőris u.35.</t>
-  </si>
-  <si>
     <t>aláírás</t>
   </si>
   <si>
     <t>………………………</t>
   </si>
   <si>
-    <t>Orczy u.  41.</t>
-  </si>
-  <si>
     <t>1089.Budapest</t>
   </si>
   <si>
@@ -81,12 +72,6 @@
     <t>Fizetendő</t>
   </si>
   <si>
-    <t>Ebéd :</t>
-  </si>
-  <si>
-    <t>Számlázandó  :</t>
-  </si>
-  <si>
     <t>[et.egysegar]</t>
   </si>
   <si>
@@ -97,6 +82,36 @@
   </si>
   <si>
     <t>[et.cim]</t>
+  </si>
+  <si>
+    <t>JSZSZGYK Gazdasági Szervezet</t>
+  </si>
+  <si>
+    <t>Kőris u. 35.</t>
+  </si>
+  <si>
+    <t>Orczy u. 41.</t>
+  </si>
+  <si>
+    <t>Ebéd H-P:</t>
+  </si>
+  <si>
+    <t>Ebéd SZ-V:</t>
+  </si>
+  <si>
+    <t>[et.adagszam_szv;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[et.fizetendo_szv]</t>
+  </si>
+  <si>
+    <t>[et.fizetendo_hp]</t>
+  </si>
+  <si>
+    <t>[et.adagszam_hp;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>Mindösszesen:</t>
   </si>
 </sst>
 </file>
@@ -249,7 +264,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="98">
+  <cellStyleXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -348,8 +363,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -398,8 +417,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="98">
+  <cellStyles count="102">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -449,6 +471,8 @@
     <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -497,6 +521,8 @@
     <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -908,7 +934,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -918,12 +944,12 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -933,12 +959,12 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -948,12 +974,12 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="7" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
       <c r="A4" s="22" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
@@ -977,7 +1003,7 @@
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1">
       <c r="A6" s="22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
@@ -1001,7 +1027,7 @@
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1">
       <c r="A8" s="23" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -1029,7 +1055,7 @@
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
       <c r="A10" s="12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="10"/>
@@ -1042,16 +1068,16 @@
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1">
       <c r="A11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>15</v>
-      </c>
       <c r="D11" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -1074,62 +1100,72 @@
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>16</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15" t="s">
+      <c r="A14" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>19</v>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17" t="s">
+        <v>28</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
       <c r="A15" s="16" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="17" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1">
       <c r="A16" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="13"/>
+        <v>30</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>19</v>
+      </c>
       <c r="C16" s="13"/>
       <c r="D16" s="21"/>
       <c r="E16" s="18" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I16" s="1"/>
     </row>
@@ -1146,7 +1182,7 @@
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1">
       <c r="A18" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1156,7 +1192,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>